<commit_message>
code modularised and made more general. More documentation is needed.
</commit_message>
<xml_diff>
--- a/test_data/fake_meta.xlsx
+++ b/test_data/fake_meta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adbennett\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBEBBDC-B3CB-48ED-8623-B4CB45E352D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF32854B-7D2E-4EE9-A859-7AD1FC9F7677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -431,9 +431,6 @@
     <t>ATTGGGTC</t>
   </si>
   <si>
-    <t>primer_#</t>
-  </si>
-  <si>
     <t>primer_id</t>
   </si>
   <si>
@@ -462,6 +459,9 @@
   </si>
   <si>
     <t>run2</t>
+  </si>
+  <si>
+    <t>primer_num</t>
   </si>
 </sst>
 </file>
@@ -841,7 +841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -852,10 +852,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" t="s">
         <v>141</v>
-      </c>
-      <c r="B1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -863,7 +863,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -871,7 +871,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -879,7 +879,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -887,7 +887,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -895,7 +895,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -903,7 +903,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -911,7 +911,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -919,7 +919,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -927,7 +927,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -935,7 +935,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -943,7 +943,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -951,7 +951,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -959,7 +959,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -967,7 +967,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -975,7 +975,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -983,7 +983,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -991,7 +991,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -999,7 +999,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -1007,7 +1007,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -1015,7 +1015,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -1023,7 +1023,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -1031,7 +1031,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -1039,7 +1039,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -1047,7 +1047,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -1055,7 +1055,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -1063,7 +1063,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -1071,7 +1071,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -1079,7 +1079,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -1087,7 +1087,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -1095,7 +1095,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -1103,7 +1103,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -1111,7 +1111,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -1119,7 +1119,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -1127,7 +1127,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -1135,7 +1135,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -1143,7 +1143,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
@@ -1151,7 +1151,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -1159,7 +1159,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
@@ -1167,7 +1167,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -1175,7 +1175,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
@@ -1183,7 +1183,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
@@ -1191,7 +1191,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -1199,7 +1199,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
@@ -1207,7 +1207,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -1215,7 +1215,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
@@ -1223,7 +1223,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
@@ -1231,7 +1231,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
@@ -1239,7 +1239,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -1247,7 +1247,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -1255,7 +1255,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
@@ -1263,7 +1263,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -1271,7 +1271,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
@@ -1279,7 +1279,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
@@ -1287,7 +1287,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -1295,7 +1295,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -1303,7 +1303,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -1311,7 +1311,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -1319,7 +1319,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
@@ -1327,7 +1327,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
@@ -1335,7 +1335,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
@@ -1343,7 +1343,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
@@ -1351,7 +1351,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
@@ -1359,7 +1359,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
@@ -1367,7 +1367,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
@@ -1375,7 +1375,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
@@ -1383,7 +1383,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
@@ -1391,7 +1391,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
@@ -1399,7 +1399,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
@@ -1407,7 +1407,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
@@ -1415,7 +1415,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
@@ -1423,7 +1423,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
@@ -1431,7 +1431,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
@@ -1439,7 +1439,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
@@ -1447,7 +1447,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
@@ -1455,7 +1455,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
@@ -1463,7 +1463,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
@@ -1471,7 +1471,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -1479,7 +1479,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
@@ -1487,7 +1487,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
@@ -1495,7 +1495,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
@@ -1503,7 +1503,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
@@ -1511,7 +1511,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
@@ -1519,7 +1519,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
@@ -1527,7 +1527,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
@@ -1535,7 +1535,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
@@ -1543,7 +1543,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
@@ -1551,7 +1551,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
@@ -1559,7 +1559,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
@@ -1567,7 +1567,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
@@ -1575,7 +1575,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
@@ -1583,7 +1583,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
@@ -1591,7 +1591,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
@@ -1599,7 +1599,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
@@ -1607,7 +1607,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -1615,7 +1615,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
@@ -1623,7 +1623,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
@@ -1631,7 +1631,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
@@ -1639,7 +1639,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
@@ -1647,7 +1647,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
@@ -1655,7 +1655,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1669,26 +1669,26 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1705,7 +1705,7 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1722,7 +1722,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1739,7 +1739,7 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1756,7 +1756,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1773,7 +1773,7 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1790,7 +1790,7 @@
         <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1807,7 +1807,7 @@
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -1824,7 +1824,7 @@
         <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -1841,7 +1841,7 @@
         <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -1858,7 +1858,7 @@
         <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -1875,7 +1875,7 @@
         <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -1892,7 +1892,7 @@
         <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -1909,7 +1909,7 @@
         <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -1926,7 +1926,7 @@
         <v>42</v>
       </c>
       <c r="E15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -1943,7 +1943,7 @@
         <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1960,7 +1960,7 @@
         <v>48</v>
       </c>
       <c r="E17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -1977,7 +1977,7 @@
         <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -1994,7 +1994,7 @@
         <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -2011,7 +2011,7 @@
         <v>57</v>
       </c>
       <c r="E20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -2028,7 +2028,7 @@
         <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -2045,7 +2045,7 @@
         <v>63</v>
       </c>
       <c r="E22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -2062,7 +2062,7 @@
         <v>66</v>
       </c>
       <c r="E23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -2079,7 +2079,7 @@
         <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -2096,7 +2096,7 @@
         <v>72</v>
       </c>
       <c r="E25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -2113,7 +2113,7 @@
         <v>75</v>
       </c>
       <c r="E26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -2130,7 +2130,7 @@
         <v>78</v>
       </c>
       <c r="E27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -2147,7 +2147,7 @@
         <v>82</v>
       </c>
       <c r="E28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -2164,7 +2164,7 @@
         <v>85</v>
       </c>
       <c r="E29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -2181,7 +2181,7 @@
         <v>88</v>
       </c>
       <c r="E30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -2198,7 +2198,7 @@
         <v>91</v>
       </c>
       <c r="E31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -2215,7 +2215,7 @@
         <v>94</v>
       </c>
       <c r="E32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -2232,7 +2232,7 @@
         <v>97</v>
       </c>
       <c r="E33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -2249,7 +2249,7 @@
         <v>100</v>
       </c>
       <c r="E34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -2266,7 +2266,7 @@
         <v>103</v>
       </c>
       <c r="E35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -2283,7 +2283,7 @@
         <v>106</v>
       </c>
       <c r="E36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -2300,7 +2300,7 @@
         <v>109</v>
       </c>
       <c r="E37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -2317,7 +2317,7 @@
         <v>112</v>
       </c>
       <c r="E38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
@@ -2334,7 +2334,7 @@
         <v>115</v>
       </c>
       <c r="E39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -2351,7 +2351,7 @@
         <v>118</v>
       </c>
       <c r="E40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -2368,7 +2368,7 @@
         <v>121</v>
       </c>
       <c r="E41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -2385,7 +2385,7 @@
         <v>124</v>
       </c>
       <c r="E42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -2402,7 +2402,7 @@
         <v>127</v>
       </c>
       <c r="E43" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
@@ -2419,7 +2419,7 @@
         <v>130</v>
       </c>
       <c r="E44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
@@ -2436,7 +2436,7 @@
         <v>133</v>
       </c>
       <c r="E45" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2448,27 +2448,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD20EFB5-BCA1-4A94-BFC2-95E1EBE40BD6}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -2485,7 +2483,7 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -2502,7 +2500,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -2519,7 +2517,7 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -2536,7 +2534,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -2553,7 +2551,7 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -2570,7 +2568,7 @@
         <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -2587,7 +2585,7 @@
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -2604,7 +2602,7 @@
         <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -2621,7 +2619,7 @@
         <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -2638,7 +2636,7 @@
         <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -2655,7 +2653,7 @@
         <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -2672,7 +2670,7 @@
         <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -2689,7 +2687,7 @@
         <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -2706,7 +2704,7 @@
         <v>42</v>
       </c>
       <c r="E15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -2723,7 +2721,7 @@
         <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -2740,7 +2738,7 @@
         <v>48</v>
       </c>
       <c r="E17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -2757,7 +2755,7 @@
         <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -2774,7 +2772,7 @@
         <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -2791,7 +2789,7 @@
         <v>57</v>
       </c>
       <c r="E20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -2808,7 +2806,7 @@
         <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -2825,7 +2823,7 @@
         <v>63</v>
       </c>
       <c r="E22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -2842,7 +2840,7 @@
         <v>66</v>
       </c>
       <c r="E23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -2859,7 +2857,7 @@
         <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -2876,7 +2874,7 @@
         <v>72</v>
       </c>
       <c r="E25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -2893,7 +2891,7 @@
         <v>75</v>
       </c>
       <c r="E26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -2910,7 +2908,7 @@
         <v>78</v>
       </c>
       <c r="E27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -2927,7 +2925,7 @@
         <v>82</v>
       </c>
       <c r="E28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -2944,7 +2942,7 @@
         <v>85</v>
       </c>
       <c r="E29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -2961,7 +2959,7 @@
         <v>88</v>
       </c>
       <c r="E30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -2978,7 +2976,7 @@
         <v>91</v>
       </c>
       <c r="E31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -2995,7 +2993,7 @@
         <v>94</v>
       </c>
       <c r="E32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -3012,7 +3010,7 @@
         <v>97</v>
       </c>
       <c r="E33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -3029,7 +3027,7 @@
         <v>100</v>
       </c>
       <c r="E34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -3046,7 +3044,7 @@
         <v>103</v>
       </c>
       <c r="E35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -3063,7 +3061,7 @@
         <v>106</v>
       </c>
       <c r="E36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -3080,7 +3078,7 @@
         <v>109</v>
       </c>
       <c r="E37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -3097,7 +3095,7 @@
         <v>112</v>
       </c>
       <c r="E38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
@@ -3114,7 +3112,7 @@
         <v>115</v>
       </c>
       <c r="E39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -3131,7 +3129,7 @@
         <v>118</v>
       </c>
       <c r="E40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -3148,7 +3146,7 @@
         <v>121</v>
       </c>
       <c r="E41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -3165,7 +3163,7 @@
         <v>124</v>
       </c>
       <c r="E42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -3182,7 +3180,7 @@
         <v>127</v>
       </c>
       <c r="E43" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
@@ -3199,7 +3197,7 @@
         <v>130</v>
       </c>
       <c r="E44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
@@ -3216,7 +3214,7 @@
         <v>133</v>
       </c>
       <c r="E45" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>